<commit_message>
fix melody chord bug
</commit_message>
<xml_diff>
--- a/Pattern_20room.xlsx
+++ b/Pattern_20room.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Duration</t>
   </si>
@@ -23,124 +23,118 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>0.25_0.5_0.75_1_0.75_0.75</t>
-  </si>
-  <si>
-    <t>71_67_73_67_71_62</t>
-  </si>
-  <si>
-    <t>1_1_0.75_0.25_0.25_0.75</t>
-  </si>
-  <si>
-    <t>73_75_75_71_70_70</t>
-  </si>
-  <si>
-    <t>2_0.75_1_0.25</t>
-  </si>
-  <si>
-    <t>77_79_79_79</t>
-  </si>
-  <si>
-    <t>0.75_0.5_0.75_2</t>
-  </si>
-  <si>
-    <t>65_67_69_76</t>
-  </si>
-  <si>
-    <t>1_0.5_1_0.5_0.25_0.5_0.25</t>
-  </si>
-  <si>
-    <t>64_73_69_74_66_62_69</t>
-  </si>
-  <si>
-    <t>0.25_1_2_0.75</t>
-  </si>
-  <si>
-    <t>78_71_68_75</t>
-  </si>
-  <si>
-    <t>1_0.75_1_0.25_1</t>
-  </si>
-  <si>
-    <t>72_69_67_74_74</t>
-  </si>
-  <si>
-    <t>0.5_0.25_0.5_2_0.75</t>
-  </si>
-  <si>
-    <t>76_76_67_67_77</t>
-  </si>
-  <si>
-    <t>0.5_1_0.75_0.25_0.25_0.25_1</t>
-  </si>
-  <si>
-    <t>64_67_66_69_66_74_66</t>
-  </si>
-  <si>
-    <t>0.75_1_0.5_0.5_0.75_0.5</t>
-  </si>
-  <si>
-    <t>71_71_73_75_73_71</t>
-  </si>
-  <si>
-    <t>1_0.25_0.5_0.5_1_0.5_0.25</t>
-  </si>
-  <si>
-    <t>72_69_79_69_67_69_69</t>
-  </si>
-  <si>
-    <t>0.25_0.75_0.5_0.5_0.5_0.75_0.75</t>
-  </si>
-  <si>
-    <t>67_74_77_76_77_77_76</t>
-  </si>
-  <si>
-    <t>0.5_0.75_1_0.25_0.5_0.25_0.75</t>
-  </si>
-  <si>
-    <t>67_71_69_69_67_67_69</t>
-  </si>
-  <si>
-    <t>1_0.25_0.5_0.75_1_0.25_0.25</t>
-  </si>
-  <si>
-    <t>78_66_68_66_71_77_71</t>
-  </si>
-  <si>
-    <t>0.5_0.75_2_0.25_0.5</t>
-  </si>
-  <si>
-    <t>79_75_67_77_69</t>
-  </si>
-  <si>
-    <t>2_2</t>
-  </si>
-  <si>
-    <t>69_70</t>
-  </si>
-  <si>
-    <t>1_0.25_0.75_1_0.5_0.25_0.25</t>
-  </si>
-  <si>
-    <t>74_64_64_71_62_64_66</t>
-  </si>
-  <si>
-    <t>1_0.5_1_0.5_0.5_0.25_0.25</t>
-  </si>
-  <si>
-    <t>75_78_77_75_78_77_71</t>
-  </si>
-  <si>
-    <t>1_0.75_1_0.5_0.25_0.25_0.25</t>
-  </si>
-  <si>
-    <t>77_77_77_74_74_69_77</t>
-  </si>
-  <si>
-    <t>1_0.5_0.25_2_0.25</t>
-  </si>
-  <si>
-    <t>67_65_72_72_77</t>
+    <t>0.75_1_1_0.75_0.5</t>
+  </si>
+  <si>
+    <t>67_71_69_65_67</t>
+  </si>
+  <si>
+    <t>0.25_0.5_0.25_1_0.25_0.25_1_0.5</t>
+  </si>
+  <si>
+    <t>69_73_69_69_64_75_64_76</t>
+  </si>
+  <si>
+    <t>1_0.25_0.25_0.5_2</t>
+  </si>
+  <si>
+    <t>73_65_68_73_77</t>
+  </si>
+  <si>
+    <t>0.25_2_0.25_0.5_0.5_0.5</t>
+  </si>
+  <si>
+    <t>74_74_65_67_67_74</t>
+  </si>
+  <si>
+    <t>2_0.5_0.75_0.75</t>
+  </si>
+  <si>
+    <t>71_62_69_60</t>
+  </si>
+  <si>
+    <t>2_1_0.25_0.75</t>
+  </si>
+  <si>
+    <t>75_68_73_64</t>
+  </si>
+  <si>
+    <t>77_65_75_65</t>
+  </si>
+  <si>
+    <t>0.75_2_0.5_0.5_0.25</t>
+  </si>
+  <si>
+    <t>68_68_67_74_75</t>
+  </si>
+  <si>
+    <t>2_0.5_0.25_0.25_0.75_0.25</t>
+  </si>
+  <si>
+    <t>72_60_72_65_71_65</t>
+  </si>
+  <si>
+    <t>0.25_0.5_1_0.25_2</t>
+  </si>
+  <si>
+    <t>75_71_75_64_69</t>
+  </si>
+  <si>
+    <t>1_1_1_0.75_0.25</t>
+  </si>
+  <si>
+    <t>72_65_72_75_77</t>
+  </si>
+  <si>
+    <t>0.25_1_0.5_2_0.25</t>
+  </si>
+  <si>
+    <t>63_72_67_72_72</t>
+  </si>
+  <si>
+    <t>0.5_0.75_1_1_0.5_0.25</t>
+  </si>
+  <si>
+    <t>71_60_69_67_60_64</t>
+  </si>
+  <si>
+    <t>0.5_0.25_1_2_0.25</t>
+  </si>
+  <si>
+    <t>76_75_64_71_64</t>
+  </si>
+  <si>
+    <t>2_0.5_1_0.25_0.25</t>
+  </si>
+  <si>
+    <t>75_73_77_68_65</t>
+  </si>
+  <si>
+    <t>0.75_0.5_0.5_0.25_2</t>
+  </si>
+  <si>
+    <t>68_74_67_65_68</t>
+  </si>
+  <si>
+    <t>0.25_2_1_0.75</t>
+  </si>
+  <si>
+    <t>69_71_64_60</t>
+  </si>
+  <si>
+    <t>2_0.5_0.25_0.75_0.5</t>
+  </si>
+  <si>
+    <t>66_64_69_75_64</t>
+  </si>
+  <si>
+    <t>2_0.25_0.5_0.25_0.25_0.75</t>
+  </si>
+  <si>
+    <t>75_65_67_75_75_65</t>
+  </si>
+  <si>
+    <t>75_67_74_68</t>
   </si>
 </sst>
 </file>
@@ -555,114 +549,114 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>